<commit_message>
Rewrote the entire script to be more legible and less code spaghetti
</commit_message>
<xml_diff>
--- a/House of Commons, Scheduler (Responses).xlsx
+++ b/House of Commons, Scheduler (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Timestamp</t>
   </si>
@@ -74,6 +74,126 @@
   </si>
   <si>
     <t>Lunch Clean, Shop, Fridges, Kitchen Deep Clean, Trash &amp; Recycling, Laundry Room and Rags, Garden Helper</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>8 AM - 9 AM, 11 AM - 12 PM, 1 PM - 2 PM, 7 PM - 8 PM</t>
+  </si>
+  <si>
+    <t>10 AM - 11 AM, 1 PM - 2 PM, 6 PM - 7 PM, 7 PM - 8 PM, 8 PM - 9 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>10 AM - 11 AM, 11 AM - 12 PM, 12 PM - 1 PM, 1 PM - 2 PM, 3 PM - 4 PM, 5 PM - 6 PM, 6 PM - 7 PM, 7 PM - 8 PM, 8 PM - 9 PM, 9 PM - 10 PM, 10 PM - 11 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 10 AM - 11 AM, 12 PM - 1 PM, 1 PM - 2 PM, 5 PM - 6 PM, 7 PM - 8 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 10 AM - 11 AM, 11 AM - 12 PM, 12 PM - 1 PM, 1 PM - 2 PM, 3 PM - 4 PM, 6 PM - 7 PM, 7 PM - 8 PM, 8 PM - 9 PM, 9 PM - 10 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>8 AM - 9 AM, 10 AM - 11 AM, 11 AM - 12 PM, 12 PM - 1 PM, 6 PM - 7 PM, 7 PM - 8 PM, 10 PM - 11 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>10 AM - 11 AM, 12 PM - 1 PM, 5 PM - 6 PM, 6 PM - 7 PM, 7 PM - 8 PM, 9 PM - 10 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>Shop, Fridges, Bathrooms, Dining Room Clean, Trash &amp; Recycling, Garden Helper</t>
+  </si>
+  <si>
+    <t>Fridges, Compost, Dining Room Clean, First Floor Commons Clean</t>
+  </si>
+  <si>
+    <t>Maddy</t>
+  </si>
+  <si>
+    <t>8 AM - 9 AM, 9 AM - 10 AM, 10 AM - 11 AM, 11 AM - 12 PM, 12 PM - 1 PM, 7 PM - 8 PM, 10 PM - 11 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>11 AM - 12 PM, 3 PM - 4 PM, 5 PM - 6 PM, 6 PM - 7 PM, 8 PM - 9 PM, 9 PM - 10 PM, 10 PM - 11 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 10 AM - 11 AM, 12 PM - 1 PM, 1 PM - 2 PM, 3 PM - 4 PM, 8 PM - 9 PM, 9 PM - 10 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 10 AM - 11 AM, 12 PM - 1 PM, 1 PM - 2 PM, 5 PM - 6 PM, 8 PM - 9 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 12 PM - 1 PM, 1 PM - 2 PM, 6 PM - 7 PM, 9 PM - 10 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>10 AM - 11 AM, 11 AM - 12 PM, 12 PM - 1 PM, 1 PM - 2 PM, 3 PM - 4 PM, 5 PM - 6 PM, 6 PM - 7 PM, 8 PM - 9 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 11 AM - 12 PM, 12 PM - 1 PM, 5 PM - 6 PM, 6 PM - 7 PM, 7 PM - 8 PM</t>
+  </si>
+  <si>
+    <t>Fast Cook, Lunch Clean, Kitchen Deep Clean, Compost, First Floor Commons Clean, Porch Yard Clean, Laundry Room and Rags, Garden Helper</t>
+  </si>
+  <si>
+    <t>Dinner Cook, Fast Cook, Fridges, Compost, Bathrooms, Porch Yard Clean</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>8 AM - 9 AM, 9 AM - 10 AM, 10 AM - 11 AM, 12 PM - 1 PM, 1 PM - 2 PM, 3 PM - 4 PM, 7 PM - 8 PM, 9 PM - 10 PM, 10 PM - 11 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>8 AM - 9 AM, 9 AM - 10 AM, 10 AM - 11 AM, 11 AM - 12 PM, 12 PM - 1 PM, 1 PM - 2 PM, 3 PM - 4 PM, 5 PM - 6 PM, 6 PM - 7 PM, 7 PM - 8 PM, 8 PM - 9 PM, 9 PM - 10 PM, 10 PM - 11 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>1 PM - 2 PM, 5 PM - 6 PM, 6 PM - 7 PM, 8 PM - 9 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>1 PM - 2 PM, 3 PM - 4 PM, 5 PM - 6 PM, 6 PM - 7 PM, 7 PM - 8 PM, 8 PM - 9 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 12 PM - 1 PM, 5 PM - 6 PM, 7 PM - 8 PM, 8 PM - 9 PM, 9 PM - 10 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>8 AM - 9 AM, 9 AM - 10 AM, 10 AM - 11 AM, 3 PM - 4 PM, 5 PM - 6 PM, 7 PM - 8 PM, 8 PM - 9 PM, 9 PM - 10 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 10 AM - 11 AM, 12 PM - 1 PM, 8 PM - 9 PM</t>
+  </si>
+  <si>
+    <t>Dinner Cook, Fast Cook, Dinner Clean, Fridges, Kitchen Deep Clean, Bathrooms, Dining Room Clean</t>
+  </si>
+  <si>
+    <t>Lunch Clean, Kitchen Deep Clean, Dining Room Clean, Pool Clean</t>
+  </si>
+  <si>
+    <t>Ada</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 11 AM - 12 PM, 12 PM - 1 PM, 6 PM - 7 PM</t>
+  </si>
+  <si>
+    <t>11 AM - 12 PM</t>
+  </si>
+  <si>
+    <t>9 AM - 10 AM, 12 PM - 1 PM, 3 PM - 4 PM, 6 PM - 7 PM, 7 PM - 8 PM, 8 PM - 9 PM, 9 PM - 10 PM, 10 PM - 11 PM, 11 PM - 12 AM</t>
+  </si>
+  <si>
+    <t>8 AM - 9 AM, 10 AM - 11 AM, 11 AM - 12 PM, 1 PM - 2 PM, 6 PM - 7 PM, 9 PM - 10 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>12 PM - 1 PM, 1 PM - 2 PM, 5 PM - 6 PM, 8 PM - 9 PM</t>
+  </si>
+  <si>
+    <t>11 AM - 12 PM, 12 PM - 1 PM, 6 PM - 7 PM, 7 PM - 8 PM, 8 PM - 9 PM, 10 PM - 11 PM</t>
+  </si>
+  <si>
+    <t>3 PM - 4 PM, 6 PM - 7 PM, 8 PM - 9 PM</t>
+  </si>
+  <si>
+    <t>Fast Cook, Dinner Clean, Kitchen Deep Clean, First Floor Commons Clean, Trash &amp; Recycling, Garden Helper</t>
+  </si>
+  <si>
+    <t>Shop, Kitchen Deep Clean, Bathrooms</t>
   </si>
 </sst>
 </file>
@@ -413,6 +533,146 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>44752.82988744213</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>44752.83030295139</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>44752.830715648146</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>44752.83098380787</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>